<commit_message>
properly sum up techs clusters
</commit_message>
<xml_diff>
--- a/bib_data/pre_1998 [Nodes].csv_cluster_totals.xlsx
+++ b/bib_data/pre_1998 [Nodes].csv_cluster_totals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
   <si>
     <t>cluster</t>
   </si>
@@ -34,22 +34,13 @@
     <t>Afforestation/reforestation</t>
   </si>
   <si>
-    <t>Soil Carbon Sequestration</t>
-  </si>
-  <si>
-    <t>BECCS</t>
+    <t>Ocean fertilisation</t>
   </si>
   <si>
     <t>Synonyms</t>
   </si>
   <si>
-    <t>Blue Carbon</t>
-  </si>
-  <si>
-    <t>Biochar</t>
-  </si>
-  <si>
-    <t>Ocean fertilisation</t>
+    <t>Soil Carbon Sequestration</t>
   </si>
   <si>
     <t>Ethics &amp; Morals</t>
@@ -61,7 +52,16 @@
     <t>Ocean Alkalinisation</t>
   </si>
   <si>
+    <t>Blue Carbon</t>
+  </si>
+  <si>
     <t>Bioenergy</t>
+  </si>
+  <si>
+    <t>Biochar</t>
+  </si>
+  <si>
+    <t>BECCS</t>
   </si>
   <si>
     <t>Direct Air Capture</t>
@@ -422,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,18 +456,18 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>81.13207547169812</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -476,18 +476,18 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>16.60377358490566</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -496,18 +496,18 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>1.132075471698113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -516,18 +516,18 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>0.3773584905660378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -536,18 +536,18 @@
         <v>9</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>0.3773584905660378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -556,18 +556,18 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0.3773584905660378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -687,42 +687,42 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>214</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>90.29535864978902</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>7.59493670886076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -733,73 +733,73 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>1.265822784810127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0.4219409282700421</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.4219409282700421</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -807,19 +807,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -847,19 +847,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -867,19 +867,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -893,13 +893,13 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -927,82 +927,82 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>37.77777777777778</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D27">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>31.74603174603174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D28">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>8.571428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>6.666666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1013,121 +1013,121 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D30">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>3.492063492063492</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D31">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>3.174603174603174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D32">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>2.857142857142857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>2.53968253968254</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>1.904761904761905</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>1.26984126984127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1153,13 +1153,13 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>315</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1167,22 +1167,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38">
-        <v>125</v>
-      </c>
-      <c r="E38">
-        <v>131</v>
-      </c>
-      <c r="F38">
-        <v>95.41984732824427</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1195,114 +1186,60 @@
       <c r="C39" t="s">
         <v>8</v>
       </c>
-      <c r="D39">
-        <v>6</v>
-      </c>
-      <c r="E39">
-        <v>131</v>
-      </c>
-      <c r="F39">
-        <v>4.580152671755725</v>
-      </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>131</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>131</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>131</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>131</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>131</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1313,16 +1250,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>131</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1333,16 +1261,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>131</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1353,16 +1272,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>131</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1373,16 +1283,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>131</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1395,34 +1296,25 @@
       <c r="C49" t="s">
         <v>5</v>
       </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>131</v>
-      </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B50">
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D50">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F50">
-        <v>86.4406779661017</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1436,70 +1328,70 @@
         <v>8</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>10.16949152542373</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B52">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F52">
-        <v>1.694915254237288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B53">
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>1.694915254237288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1507,19 +1399,19 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -1533,13 +1425,13 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1553,13 +1445,13 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -1573,13 +1465,13 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>0</v>
       </c>
       <c r="E58">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1593,13 +1485,13 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="E59">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -1613,13 +1505,13 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1639,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -1647,87 +1539,51 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
-      </c>
-      <c r="D62">
-        <v>66</v>
-      </c>
-      <c r="E62">
-        <v>81</v>
-      </c>
-      <c r="F62">
-        <v>81.48148148148148</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63">
-        <v>7</v>
-      </c>
-      <c r="E63">
-        <v>81</v>
-      </c>
-      <c r="F63">
-        <v>8.641975308641975</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
-      </c>
-      <c r="D64">
-        <v>6</v>
-      </c>
-      <c r="E64">
-        <v>81</v>
-      </c>
-      <c r="F64">
-        <v>7.407407407407407</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" s="1">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <v>81</v>
-      </c>
-      <c r="F65">
-        <v>1.234567901234568</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>6</v>
@@ -1735,394 +1591,82 @@
       <c r="C66" t="s">
         <v>16</v>
       </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66">
-        <v>81</v>
-      </c>
-      <c r="F66">
-        <v>1.234567901234568</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="1">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>6</v>
       </c>
       <c r="C67" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
         <v>12</v>
       </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>81</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="1">
-        <v>63</v>
-      </c>
-      <c r="B68">
-        <v>6</v>
-      </c>
-      <c r="C68" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>81</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="1">
-        <v>64</v>
-      </c>
-      <c r="B69">
-        <v>6</v>
-      </c>
-      <c r="C69" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>81</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="1">
-        <v>65</v>
-      </c>
-      <c r="B70">
-        <v>6</v>
-      </c>
-      <c r="C70" t="s">
-        <v>13</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>81</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="1">
-        <v>66</v>
-      </c>
-      <c r="B71">
-        <v>6</v>
-      </c>
-      <c r="C71" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>81</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="1">
-        <v>67</v>
-      </c>
-      <c r="B72">
-        <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>81</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>81</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="1">
-        <v>80</v>
-      </c>
-      <c r="B74">
         <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74">
-        <v>2</v>
-      </c>
-      <c r="E74">
-        <v>2</v>
-      </c>
-      <c r="F74">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="1">
-        <v>72</v>
-      </c>
-      <c r="B75">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>2</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="1">
-        <v>73</v>
-      </c>
-      <c r="B76">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>2</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="1">
-        <v>74</v>
-      </c>
-      <c r="B77">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>2</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="1">
-        <v>75</v>
-      </c>
-      <c r="B78">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>2</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="1">
-        <v>76</v>
-      </c>
-      <c r="B79">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>2</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="1">
-        <v>77</v>
-      </c>
-      <c r="B80">
-        <v>7</v>
-      </c>
-      <c r="C80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>2</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="1">
-        <v>78</v>
-      </c>
-      <c r="B81">
-        <v>7</v>
-      </c>
-      <c r="C81" t="s">
-        <v>10</v>
-      </c>
-      <c r="D81">
-        <v>0</v>
-      </c>
-      <c r="E81">
-        <v>2</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="1">
-        <v>79</v>
-      </c>
-      <c r="B82">
-        <v>7</v>
-      </c>
-      <c r="C82" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>2</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="1">
-        <v>81</v>
-      </c>
-      <c r="B83">
-        <v>7</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83">
-        <v>0</v>
-      </c>
-      <c r="E83">
-        <v>2</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="1">
-        <v>82</v>
-      </c>
-      <c r="B84">
-        <v>7</v>
-      </c>
-      <c r="C84" t="s">
-        <v>9</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>2</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="1">
-        <v>83</v>
-      </c>
-      <c r="B85">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>2</v>
-      </c>
-      <c r="F85">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
properly sum up techs, for real
</commit_message>
<xml_diff>
--- a/bib_data/pre_1998 [Nodes].csv_cluster_totals.xlsx
+++ b/bib_data/pre_1998 [Nodes].csv_cluster_totals.xlsx
@@ -43,13 +43,13 @@
     <t>Soil Carbon Sequestration</t>
   </si>
   <si>
+    <t>Ocean Alkalinisation</t>
+  </si>
+  <si>
     <t>Ethics &amp; Morals</t>
   </si>
   <si>
     <t>Enhanced Weathering</t>
-  </si>
-  <si>
-    <t>Ocean Alkalinisation</t>
   </si>
   <si>
     <t>Blue Carbon</t>
@@ -456,13 +456,13 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>50</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -476,13 +476,13 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>50</v>
+        <v>33.33333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -496,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>11.11111111111111</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -516,18 +516,18 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>11.11111111111111</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -536,18 +536,18 @@
         <v>9</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>11.11111111111111</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -579,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -619,7 +619,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -639,7 +639,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -679,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -696,10 +696,10 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F14">
         <v>100</v>
@@ -713,13 +713,13 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -793,13 +793,13 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -813,13 +813,13 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -899,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -936,10 +936,10 @@
         <v>5</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F26">
         <v>100</v>
@@ -953,13 +953,13 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1013,13 +1013,13 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1033,13 +1033,13 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1167,13 +1167,22 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1186,32 +1195,59 @@
       <c r="C39" t="s">
         <v>8</v>
       </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>25</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -1219,10 +1255,19 @@
       <c r="C42" t="s">
         <v>9</v>
       </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1230,71 +1275,134 @@
       <c r="C43" t="s">
         <v>10</v>
       </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1308,10 +1416,10 @@
         <v>5</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F50">
         <v>100</v>
@@ -1331,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -1351,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -1371,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -1385,13 +1493,13 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -1405,13 +1513,13 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -1425,13 +1533,13 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -1451,7 +1559,7 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -1471,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -1491,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -1511,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -1531,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -1539,29 +1647,47 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B62">
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>6</v>
@@ -1569,10 +1695,19 @@
       <c r="C64" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>6</v>
@@ -1580,63 +1715,117 @@
       <c r="C65" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1646,8 +1835,17 @@
       <c r="C71" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1657,8 +1855,17 @@
       <c r="C72" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1667,6 +1874,15 @@
       </c>
       <c r="C73" t="s">
         <v>7</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>